<commit_message>
SSDM-13256: Added missing columns for experiment types.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment-type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment-type.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t xml:space="preserve">EXPERIMENT_TYPE</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Validation script</t>
   </si>
   <si>
+    <t xml:space="preserve">Modification Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEFAULT_EXPERIMENT</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">test.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-11 17:23:44</t>
   </si>
   <si>
     <t xml:space="preserve">Mandatory</t>
@@ -122,8 +128,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -204,7 +211,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -218,6 +225,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,7 +252,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -261,16 +272,22 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,131 +295,131 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>

</xml_diff>